<commit_message>
Update to dictionary for skips and POIs
</commit_message>
<xml_diff>
--- a/data-raw/dictionary.xlsx
+++ b/data-raw/dictionary.xlsx
@@ -1,106 +1,152 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Malawi_project\Phase 2\wasteskipsblantyre\data-raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ACD911-1E6F-474A-A754-5A7283FA21F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="28680" yWindow="-10290" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
-  <si>
-    <t xml:space="preserve">directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">file_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">variable_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skips.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">name_other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">supervision_area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">context</t>
-  </si>
-  <si>
-    <t xml:space="preserve">direct_access</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fillup</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fillup_dry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fillup_rainy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number_skips</t>
-  </si>
-  <si>
-    <t xml:space="preserve">capacity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">poi.rda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">poi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">long</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
+  <si>
+    <t>directory</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>variable_name</t>
+  </si>
+  <si>
+    <t>variable_type</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>data/</t>
+  </si>
+  <si>
+    <t>skips.rda</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>character</t>
+  </si>
+  <si>
+    <t>name_other</t>
+  </si>
+  <si>
+    <t>supervision_area</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>direct_access</t>
+  </si>
+  <si>
+    <t>fillup</t>
+  </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>fillup_dry</t>
+  </si>
+  <si>
+    <t>fillup_rainy</t>
+  </si>
+  <si>
+    <t>number_skips</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>poi.rda</t>
+  </si>
+  <si>
+    <t>poi</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>Main name of skip location.</t>
+  </si>
+  <si>
+    <t>Cleansing supervision area.</t>
+  </si>
+  <si>
+    <t>Type of urban environment surrounding skip location.</t>
+  </si>
+  <si>
+    <t>Vehicle access path type.</t>
+  </si>
+  <si>
+    <t>Number of days to fill up according to person surveyed.</t>
+  </si>
+  <si>
+    <t>Number of days to fill up in dry season according to person surveyed.</t>
+  </si>
+  <si>
+    <t>Number of days to fill up in rainy season according to person surveyed.</t>
+  </si>
+  <si>
+    <t>Capacity in m3.</t>
+  </si>
+  <si>
+    <t>Number of skips at skip location.</t>
+  </si>
+  <si>
+    <t>Y (latitude) coordinate in WGS 84.</t>
+  </si>
+  <si>
+    <t>X (longitude) coordinate in WGS 84.</t>
+  </si>
+  <si>
+    <t>Notes relating to skip location.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point of interest. </t>
+  </si>
+  <si>
+    <t>Alternative names of skip location separated by commas.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -136,6 +182,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -417,14 +472,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="11.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +501,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -455,27 +515,27 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -483,16 +543,16 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -500,16 +560,16 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -517,16 +577,16 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -534,187 +594,187 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>19</v>
       </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
         <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
       <c r="D17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>